<commit_message>
Update Rizka-Simulasi dan Pengajuan Kredit Mobil Baru Paket dan Nonpaket
</commit_message>
<xml_diff>
--- a/SimulasiKreditMobilBaru.xlsx
+++ b/SimulasiKreditMobilBaru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59373D9A-17FA-4344-B046-265DCAEF9D30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202AABD5-FC0A-4077-B018-88C4C69B217E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6105" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="1" xr2:uid="{706A06F3-AF32-444F-ACFA-922EC4B407C6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
   <si>
     <t>namaCabang</t>
   </si>
@@ -93,13 +93,34 @@
     <t>namaPaketBaru</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>ACC ANNIVERSARY</t>
+  </si>
+  <si>
+    <t>paket</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>catatan</t>
+  </si>
+  <si>
+    <t>agreeTermsAndCondition</t>
+  </si>
+  <si>
+    <t>Aku Cinta ACC</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Daihatsu</t>
+  </si>
+  <si>
+    <t>TOYOTA YARIS TRD SPORTIVO</t>
+  </si>
+  <si>
+    <t>DAIHATSU NEW AYLA 1.0 D M/T 2019</t>
   </si>
 </sst>
 </file>
@@ -190,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -226,6 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1998,165 +2022,346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30B3FC-28D1-42D3-B965-D4269AC997F7}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="M1" s="14"/>
+    </row>
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="F2" s="3">
         <v>16</v>
       </c>
-      <c r="E2" s="3">
+      <c r="G2" s="3">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="3">
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="3">
         <v>16</v>
       </c>
-      <c r="E3" s="3">
+      <c r="G3" s="3">
         <v>24</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="F4" s="3">
         <v>25</v>
       </c>
-      <c r="E4" s="3">
+      <c r="G4" s="3">
         <v>48</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
         <v>25</v>
       </c>
-      <c r="E5" s="3">
+      <c r="G5" s="3">
         <v>48</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="J5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3">
+        <v>24</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3">
+        <v>24</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3">
+        <v>48</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3">
+        <v>48</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Rizka - Simulasi Kredit Mobil Baru
</commit_message>
<xml_diff>
--- a/SimulasiKreditMobilBaru.xlsx
+++ b/SimulasiKreditMobilBaru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202AABD5-FC0A-4077-B018-88C4C69B217E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F97524E-E9E4-4A53-98B7-17AA4586EE49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="1" xr2:uid="{706A06F3-AF32-444F-ACFA-922EC4B407C6}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="1" xr2:uid="{706A06F3-AF32-444F-ACFA-922EC4B407C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
   <si>
     <t>namaCabang</t>
   </si>
@@ -93,9 +93,6 @@
     <t>namaPaketBaru</t>
   </si>
   <si>
-    <t>ACC ANNIVERSARY</t>
-  </si>
-  <si>
     <t>paket</t>
   </si>
   <si>
@@ -117,17 +114,26 @@
     <t>Daihatsu</t>
   </si>
   <si>
-    <t>TOYOTA YARIS TRD SPORTIVO</t>
-  </si>
-  <si>
     <t>DAIHATSU NEW AYLA 1.0 D M/T 2019</t>
+  </si>
+  <si>
+    <t>TOYOTA KIJANG INNOVA 2020</t>
+  </si>
+  <si>
+    <t>TOYOTA AGYA</t>
+  </si>
+  <si>
+    <t>kurangDari20Persen</t>
+  </si>
+  <si>
+    <t>TOYOTA RUSH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +162,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2022,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30B3FC-28D1-42D3-B965-D4269AC997F7}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,15 +2052,15 @@
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>15</v>
@@ -2071,10 +2084,10 @@
         <v>6</v>
       </c>
       <c r="J1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>10</v>
@@ -2087,16 +2100,14 @@
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="E2" s="15"/>
       <c r="F2" s="3">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3">
         <v>24</v>
@@ -2108,7 +2119,7 @@
         <v>13</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>9</v>
@@ -2124,14 +2135,12 @@
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="15"/>
       <c r="F3" s="3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>24</v>
@@ -2143,7 +2152,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>9</v>
@@ -2159,16 +2168,12 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>19</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3">
         <v>48</v>
@@ -2180,7 +2185,7 @@
         <v>9</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>9</v>
@@ -2196,16 +2201,14 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="E5" s="15"/>
       <c r="F5" s="3">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3">
         <v>48</v>
@@ -2217,7 +2220,7 @@
         <v>13</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>9</v>
@@ -2232,15 +2235,15 @@
         <v>13</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>24</v>
@@ -2252,7 +2255,7 @@
         <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>9</v>
@@ -2266,15 +2269,15 @@
         <v>13</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G7" s="3">
         <v>24</v>
@@ -2286,7 +2289,7 @@
         <v>9</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>9</v>
@@ -2300,10 +2303,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2320,50 +2323,17 @@
         <v>9</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3">
-        <v>25</v>
-      </c>
-      <c r="G9" s="3">
-        <v>48</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>14</v>
+      <c r="L8" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Rizka - Simulasi dan Pengajuan Kredit Mobil Baru Paket NonPaket
</commit_message>
<xml_diff>
--- a/SimulasiKreditMobilBaru.xlsx
+++ b/SimulasiKreditMobilBaru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E930210B-514E-4296-973C-F612D2462012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711CCC36-95F9-4A41-B2A2-4E9CFA9D0049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="1" xr2:uid="{706A06F3-AF32-444F-ACFA-922EC4B407C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{706A06F3-AF32-444F-ACFA-922EC4B407C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2084,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30B3FC-28D1-42D3-B965-D4269AC997F7}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="27">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G5" s="27">
         <v>48</v>
@@ -2290,7 +2290,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="24">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G6" s="24">
         <v>24</v>

</xml_diff>